<commit_message>
Gráfico de barra com variação de cor
</commit_message>
<xml_diff>
--- a/7-Gráficos/27. Gráfico de Acompanhamento de Meta - Material(1).xlsx
+++ b/7-Gráficos/27. Gráfico de Acompanhamento de Meta - Material(1).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damor\Dropbox\Hashtag (1)\Hashtag\Online\Conteúdos\Planilhas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\cursos\excel\7-Gráficos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D50E2334-CD56-4C35-B5E4-599814BFC57D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A1BB8FA-3326-4D78-B66B-4EA26C51EC1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{41202370-5C6F-4C36-8D7A-1715839ED562}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{41202370-5C6F-4C36-8D7A-1715839ED562}"/>
   </bookViews>
   <sheets>
     <sheet name="Gabarito" sheetId="1" r:id="rId1"/>
@@ -24,15 +24,23 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="7">
   <si>
     <t>Data</t>
   </si>
@@ -51,6 +59,9 @@
   <si>
     <t>Meta Restante</t>
   </si>
+  <si>
+    <t>Meta ano</t>
+  </si>
 </sst>
 </file>
 
@@ -58,7 +69,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -126,14 +137,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
@@ -570,7 +582,510 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Do zero'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Fat. Acum.</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Do zero'!$A$2:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\-yy</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>43466</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43497</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43525</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43556</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43586</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43617</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43647</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43678</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43709</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>43739</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43770</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>43800</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Do zero'!$C$2:$C$13</c:f>
+              <c:numCache>
+                <c:formatCode>_-"R$"\ * #,##0_-;\-"R$"\ * #,##0_-;_-"R$"\ * "-"??_-;_-@_-</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>58000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>102000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>114000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>141000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>216000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>231000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>245000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>345000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>398000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>455000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-79E5-4843-BBD1-6A3A4F0A87FF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Do zero'!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Meta Restante</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Do zero'!$A$2:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\-yy</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>43466</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43497</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43525</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43556</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43586</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43617</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43647</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43678</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43709</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>43739</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43770</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>43800</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Do zero'!$F$2:$F$13</c:f>
+              <c:numCache>
+                <c:formatCode>_-"$"\ * #.##0_-;\-"$"\ * #.##0_-;_-"$"\ * "-"??_-;_-@_-</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>510000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>472000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>488000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>428000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>416000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>389000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>314000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>299000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>285000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>185000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>132000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>75000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-79E5-4843-BBD1-6A3A4F0A87FF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="1019728464"/>
+        <c:axId val="1019728944"/>
+      </c:barChart>
+      <c:dateAx>
+        <c:axId val="1019728464"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="mmm\-yy" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1019728944"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="months"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="1019728944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1019728464"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1081,6 +1596,511 @@
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -1154,10 +2174,51 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>138111</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Gráfico 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CEDB62CF-7A74-AF50-A2C7-14343ACBDEF9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1195,7 +2256,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1301,7 +2362,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1443,7 +2504,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1453,8 +2514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A4839BE-0558-4CCA-845C-378736781985}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1771,16 +2832,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4713B566-117B-4EE8-97E5-5DC4BAF7B148}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F13"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
@@ -1814,12 +2875,18 @@
       <c r="B2" s="3">
         <v>20000</v>
       </c>
-      <c r="C2" s="3"/>
+      <c r="C2" s="3">
+        <f>B2</f>
+        <v>20000</v>
+      </c>
       <c r="D2" s="3">
         <v>34000</v>
       </c>
       <c r="E2" s="3"/>
-      <c r="F2" s="4"/>
+      <c r="F2" s="4">
+        <f>$B$15-C2</f>
+        <v>510000</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
@@ -1828,12 +2895,18 @@
       <c r="B3" s="3">
         <v>38000</v>
       </c>
-      <c r="C3" s="3"/>
+      <c r="C3" s="3">
+        <f>C2 + B3</f>
+        <v>58000</v>
+      </c>
       <c r="D3" s="3">
         <v>17000</v>
       </c>
       <c r="E3" s="3"/>
-      <c r="F3" s="4"/>
+      <c r="F3" s="4">
+        <f t="shared" ref="F3:F13" si="0">$B$15-C3</f>
+        <v>472000</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
@@ -1842,12 +2915,18 @@
       <c r="B4" s="3">
         <v>25000</v>
       </c>
-      <c r="C4" s="3"/>
+      <c r="C4" s="3">
+        <f>D3 + B4</f>
+        <v>42000</v>
+      </c>
       <c r="D4" s="3">
         <v>11000</v>
       </c>
       <c r="E4" s="3"/>
-      <c r="F4" s="4"/>
+      <c r="F4" s="4">
+        <f t="shared" si="0"/>
+        <v>488000</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
@@ -1856,12 +2935,18 @@
       <c r="B5" s="3">
         <v>60000</v>
       </c>
-      <c r="C5" s="3"/>
+      <c r="C5" s="3">
+        <f xml:space="preserve"> C4 + B5</f>
+        <v>102000</v>
+      </c>
       <c r="D5" s="3">
         <v>25000</v>
       </c>
       <c r="E5" s="3"/>
-      <c r="F5" s="4"/>
+      <c r="F5" s="4">
+        <f t="shared" si="0"/>
+        <v>428000</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
@@ -1870,12 +2955,18 @@
       <c r="B6" s="3">
         <v>12000</v>
       </c>
-      <c r="C6" s="3"/>
+      <c r="C6" s="3">
+        <f xml:space="preserve"> C5 + B6</f>
+        <v>114000</v>
+      </c>
       <c r="D6" s="3">
         <v>50000</v>
       </c>
       <c r="E6" s="3"/>
-      <c r="F6" s="4"/>
+      <c r="F6" s="4">
+        <f t="shared" si="0"/>
+        <v>416000</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
@@ -1884,12 +2975,18 @@
       <c r="B7" s="3">
         <v>27000</v>
       </c>
-      <c r="C7" s="3"/>
+      <c r="C7" s="3">
+        <f xml:space="preserve"> C6 + B7</f>
+        <v>141000</v>
+      </c>
       <c r="D7" s="3">
         <v>50000</v>
       </c>
       <c r="E7" s="3"/>
-      <c r="F7" s="4"/>
+      <c r="F7" s="4">
+        <f t="shared" si="0"/>
+        <v>389000</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
@@ -1898,12 +2995,18 @@
       <c r="B8" s="3">
         <v>75000</v>
       </c>
-      <c r="C8" s="3"/>
+      <c r="C8" s="3">
+        <f xml:space="preserve"> C7 + B8</f>
+        <v>216000</v>
+      </c>
       <c r="D8" s="3">
         <v>35000</v>
       </c>
       <c r="E8" s="3"/>
-      <c r="F8" s="4"/>
+      <c r="F8" s="4">
+        <f t="shared" si="0"/>
+        <v>314000</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
@@ -1912,12 +3015,18 @@
       <c r="B9" s="3">
         <v>15000</v>
       </c>
-      <c r="C9" s="3"/>
+      <c r="C9" s="3">
+        <f xml:space="preserve"> C8 + B9</f>
+        <v>231000</v>
+      </c>
       <c r="D9" s="3">
         <v>61000</v>
       </c>
       <c r="E9" s="3"/>
-      <c r="F9" s="4"/>
+      <c r="F9" s="4">
+        <f t="shared" si="0"/>
+        <v>299000</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
@@ -1926,12 +3035,18 @@
       <c r="B10" s="3">
         <v>14000</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="3">
+        <f xml:space="preserve"> C9 + B10</f>
+        <v>245000</v>
+      </c>
       <c r="D10" s="3">
         <v>83000</v>
       </c>
       <c r="E10" s="3"/>
-      <c r="F10" s="4"/>
+      <c r="F10" s="4">
+        <f t="shared" si="0"/>
+        <v>285000</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
@@ -1940,12 +3055,18 @@
       <c r="B11" s="3">
         <v>100000</v>
       </c>
-      <c r="C11" s="3"/>
+      <c r="C11" s="3">
+        <f xml:space="preserve"> C10 + B11</f>
+        <v>345000</v>
+      </c>
       <c r="D11" s="3">
         <v>23000</v>
       </c>
       <c r="E11" s="3"/>
-      <c r="F11" s="4"/>
+      <c r="F11" s="4">
+        <f t="shared" si="0"/>
+        <v>185000</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
@@ -1954,12 +3075,18 @@
       <c r="B12" s="3">
         <v>53000</v>
       </c>
-      <c r="C12" s="3"/>
+      <c r="C12" s="3">
+        <f t="shared" ref="C6:C13" si="1" xml:space="preserve"> C11 + B12</f>
+        <v>398000</v>
+      </c>
       <c r="D12" s="3">
         <v>92000</v>
       </c>
       <c r="E12" s="3"/>
-      <c r="F12" s="4"/>
+      <c r="F12" s="4">
+        <f t="shared" si="0"/>
+        <v>132000</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
@@ -1968,14 +3095,29 @@
       <c r="B13" s="3">
         <v>57000</v>
       </c>
-      <c r="C13" s="3"/>
+      <c r="C13" s="3">
+        <f t="shared" si="1"/>
+        <v>455000</v>
+      </c>
       <c r="D13" s="3">
         <v>49000</v>
       </c>
       <c r="E13" s="3"/>
-      <c r="F13" s="4"/>
+      <c r="F13" s="4">
+        <f t="shared" si="0"/>
+        <v>75000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="5">
+        <v>530000</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>